<commit_message>
barra de busqueda arreglos en las vistas
</commit_message>
<xml_diff>
--- a/app/tmp/reporte_ovejas.xlsx
+++ b/app/tmp/reporte_ovejas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,11 +480,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>aleja</t>
+          <t>lacy</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>38353</v>
+        <v>45546</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -493,11 +493,63 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hembra</t>
+          <t>Macho</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>lacy</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45546</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>dorper</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Macho</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lacy</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45546</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>dorper</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Macho</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>